<commit_message>
fixed typo in cleaning code
</commit_message>
<xml_diff>
--- a/Raw Data/State Data/States.xlsx
+++ b/Raw Data/State Data/States.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/96cc1363e59f2cdc/Data_Analysis_bootcamp/Module_20/dexter_project/Data/State Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/96cc1363e59f2cdc/Data_Analysis_bootcamp/Module_20/dexter_project/Raw Data/State Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A5FFE839-7F04-46A3-8CE4-4A712F5A237C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="8_{A5FFE839-7F04-46A3-8CE4-4A712F5A237C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5634D0A3-98EA-4700-B475-0AE564D88826}"/>
   <bookViews>
-    <workbookView xWindow="3465" yWindow="1980" windowWidth="21210" windowHeight="16590" xr2:uid="{58E46EDE-15B7-44C7-94B1-44C1CC0AE84F}"/>
+    <workbookView xWindow="7305" yWindow="3450" windowWidth="21210" windowHeight="16590" xr2:uid="{58E46EDE-15B7-44C7-94B1-44C1CC0AE84F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="61">
   <si>
     <t>Name</t>
   </si>
@@ -209,6 +209,15 @@
   </si>
   <si>
     <t>West</t>
+  </si>
+  <si>
+    <t>U.S. Virgin Islands</t>
+  </si>
+  <si>
+    <t>Noncontinental</t>
+  </si>
+  <si>
+    <t>Puerto Rico</t>
   </si>
 </sst>
 </file>
@@ -572,10 +581,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83EE7814-E97A-4DD5-BE8E-5DE27263B1C8}">
-  <dimension ref="A1:B52"/>
+  <dimension ref="A1:B55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H42" sqref="H42"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -744,7 +753,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>22</v>
       </c>
@@ -752,7 +761,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>23</v>
       </c>
@@ -760,7 +769,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>24</v>
       </c>
@@ -768,7 +777,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>25</v>
       </c>
@@ -776,7 +785,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>26</v>
       </c>
@@ -784,7 +793,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>28</v>
       </c>
@@ -792,7 +801,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>29</v>
       </c>
@@ -856,7 +865,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>37</v>
       </c>
@@ -864,7 +873,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>38</v>
       </c>
@@ -872,7 +881,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>39</v>
       </c>
@@ -880,7 +889,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>41</v>
       </c>
@@ -888,7 +897,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>42</v>
       </c>
@@ -896,7 +905,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>43</v>
       </c>
@@ -904,7 +913,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>44</v>
       </c>
@@ -912,7 +921,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>46</v>
       </c>
@@ -984,7 +993,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>55</v>
       </c>
@@ -992,13 +1001,32 @@
         <v>57</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>56</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>57</v>
       </c>
+    </row>
+    <row r="53" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fixed missing data in raw
</commit_message>
<xml_diff>
--- a/Raw Data/State Data/States.xlsx
+++ b/Raw Data/State Data/States.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/96cc1363e59f2cdc/Data_Analysis_bootcamp/Module_20/dexter_project/Raw Data/State Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{A5FFE839-7F04-46A3-8CE4-4A712F5A237C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5634D0A3-98EA-4700-B475-0AE564D88826}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="8_{A5FFE839-7F04-46A3-8CE4-4A712F5A237C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7D901795-6818-49E3-A782-A260B20BEA43}"/>
   <bookViews>
-    <workbookView xWindow="7305" yWindow="3450" windowWidth="21210" windowHeight="16590" xr2:uid="{58E46EDE-15B7-44C7-94B1-44C1CC0AE84F}"/>
+    <workbookView xWindow="18720" yWindow="2655" windowWidth="19140" windowHeight="16425" xr2:uid="{58E46EDE-15B7-44C7-94B1-44C1CC0AE84F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$54</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -35,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="105">
   <si>
     <t>Name</t>
   </si>
@@ -218,6 +221,138 @@
   </si>
   <si>
     <t>Puerto Rico</t>
+  </si>
+  <si>
+    <t>Florida                149704</t>
+  </si>
+  <si>
+    <t>New York                97043</t>
+  </si>
+  <si>
+    <t>Texas                   75053</t>
+  </si>
+  <si>
+    <t>North Carolina          66263</t>
+  </si>
+  <si>
+    <t>Georgia                 63377</t>
+  </si>
+  <si>
+    <t>Illinois                57487</t>
+  </si>
+  <si>
+    <t>Massachusetts           48030</t>
+  </si>
+  <si>
+    <t>California              46907</t>
+  </si>
+  <si>
+    <t>Ohio                    37326</t>
+  </si>
+  <si>
+    <t>Michigan                32792</t>
+  </si>
+  <si>
+    <t>Tennessee               32412</t>
+  </si>
+  <si>
+    <t>South Carolina          31672</t>
+  </si>
+  <si>
+    <t>Pennsylvania            30472</t>
+  </si>
+  <si>
+    <t>Colorado                28658</t>
+  </si>
+  <si>
+    <t>Virginia                25922</t>
+  </si>
+  <si>
+    <t>Missouri                25908</t>
+  </si>
+  <si>
+    <t>Kentucky                25141</t>
+  </si>
+  <si>
+    <t>Minnesota               19398</t>
+  </si>
+  <si>
+    <t>Rhode Island            18467</t>
+  </si>
+  <si>
+    <t>Connecticut             17427</t>
+  </si>
+  <si>
+    <t>New Jersey              17040</t>
+  </si>
+  <si>
+    <t>Maine                   16752</t>
+  </si>
+  <si>
+    <t>Indiana                 13651</t>
+  </si>
+  <si>
+    <t>Louisiana               13332</t>
+  </si>
+  <si>
+    <t>Nevada                  11457</t>
+  </si>
+  <si>
+    <t>New Hampshire           10942</t>
+  </si>
+  <si>
+    <t>Washington              10677</t>
+  </si>
+  <si>
+    <t>Alabama                  9773</t>
+  </si>
+  <si>
+    <t>Arizona                  9369</t>
+  </si>
+  <si>
+    <t>Vermont                  6520</t>
+  </si>
+  <si>
+    <t>Puerto Rico              6275</t>
+  </si>
+  <si>
+    <t>Wisconsin                6113</t>
+  </si>
+  <si>
+    <t>Utah                     5079</t>
+  </si>
+  <si>
+    <t>West Virginia            3914</t>
+  </si>
+  <si>
+    <t>Oklahoma                 3354</t>
+  </si>
+  <si>
+    <t>Oregon                   2112</t>
+  </si>
+  <si>
+    <t>Nebraska                 1902</t>
+  </si>
+  <si>
+    <t>Arkansas                 1796</t>
+  </si>
+  <si>
+    <t>Iowa                     1564</t>
+  </si>
+  <si>
+    <t>New Mexico               1402</t>
+  </si>
+  <si>
+    <t>Mississippi              1248</t>
+  </si>
+  <si>
+    <t>U.S. Virgin Islands       758</t>
+  </si>
+  <si>
+    <t>Hawaii                    575</t>
+  </si>
+  <si>
+    <t>Montana                    69</t>
   </si>
 </sst>
 </file>
@@ -581,10 +716,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83EE7814-E97A-4DD5-BE8E-5DE27263B1C8}">
-  <dimension ref="A1:B55"/>
+  <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,7 +728,7 @@
     <col min="2" max="2" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -601,434 +736,569 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="D2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>8</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="2" t="s">
+      <c r="D20" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="D22" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="B25" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="D27" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="D29" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="D30" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="D31" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="D32" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="D33" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="D34" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D37" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D38" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D39" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D40" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D41" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D42" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B43" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B38" s="2" t="s">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D44" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D45" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="D46" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D47" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>52</v>
+        <v>5</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="D48" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>53</v>
+        <v>16</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="D49" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D50" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D52" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D53" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B54" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D1:D55">
+    <sortCondition ref="D1:D55"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>